<commit_message>
conducted more test and added to excel file
</commit_message>
<xml_diff>
--- a/Design Test.xlsx
+++ b/Design Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segre\Desktop\Progetto_ISS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AF908B-8021-4011-B018-5B109B33B2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C1B493-87C3-408A-BE63-4D73A300B4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="249">
   <si>
     <t>ID Test</t>
   </si>
@@ -575,13 +575,1837 @@
   </si>
   <si>
     <t>Stato del Drago con HP = 0.</t>
+  </si>
+  <si>
+    <t>TC-13</t>
+  </si>
+  <si>
+    <t>test_draft_monster_selection</t>
+  </si>
+  <si>
+    <t>TC-14</t>
+  </si>
+  <si>
+    <t>TC-15</t>
+  </si>
+  <si>
+    <t>TC-16</t>
+  </si>
+  <si>
+    <t>TC-17</t>
+  </si>
+  <si>
+    <t>TC-18</t>
+  </si>
+  <si>
+    <t>TC-19</t>
+  </si>
+  <si>
+    <t>TC-20</t>
+  </si>
+  <si>
+    <t>TC-21</t>
+  </si>
+  <si>
+    <t>test_forced_switch_on_death</t>
+  </si>
+  <si>
+    <t>TC-22</t>
+  </si>
+  <si>
+    <t>TC-23</t>
+  </si>
+  <si>
+    <r>
+      <t>ChooseDraft('Serpe').execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>game.turn = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il mostro 'Serpe' viene aggiunto a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>game.teams[0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Il turno cambia (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>game.turn = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Serpe aggiunto, turno 1</t>
+  </si>
+  <si>
+    <t>test_team_limit_selection</t>
+  </si>
+  <si>
+    <r>
+      <t>SetTeamLimitAction(3).execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.team_limit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> impostato a 3. Il menu attivo diventa 'draft'.</t>
+    </r>
+  </si>
+  <si>
+    <t>3, 'draft'</t>
+  </si>
+  <si>
+    <t>test_xp_gain_and_plus_activation</t>
+  </si>
+  <si>
+    <t>Il team 0 ha 2 XP e usa una mossa che dà 1 XP.</t>
+  </si>
+  <si>
+    <r>
+      <t>game.teams_xp[0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> raggiunge 3. Si attiva </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>active_plus_durations[0] = 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Plus Attivo</t>
+  </si>
+  <si>
+    <t>test_plus_move_scaling</t>
+  </si>
+  <si>
+    <t>Drago in modalità Plus usa "Palla di fuoco+".</t>
+  </si>
+  <si>
+    <t>Viene usata la versione Plus della mossa con potenza aumentata (es. +30 danno extra).</t>
+  </si>
+  <si>
+    <t>Danno aumentato</t>
+  </si>
+  <si>
+    <t>test_status_effect_debuff</t>
+  </si>
+  <si>
+    <t>Uso di "Calura" (Debuff Difesa 50% per 2 turni).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il target riceve un </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>Status_effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>power = -0.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nella lista </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>status_effects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Effetto presente</t>
+  </si>
+  <si>
+    <t>test_stat_recalculation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mostro con Attacco 100 e Buff Attacco 20%. Chiamata a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>update_status_effects()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La statistica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>self.attack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> del mostro viene ricalcolata a 120.</t>
+    </r>
+  </si>
+  <si>
+    <t>test_plus_remove_debuffs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Esecuzione </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>PlusRemoveDebuffs.activate()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> su un mostro con debuff attivi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tutti gli effetti con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>power &lt; 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> vengono rimossi dalla lista </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>status_effects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Debuff rimossi</t>
+  </si>
+  <si>
+    <t>test_win_condition</t>
+  </si>
+  <si>
+    <r>
+      <t>remove_monster_from_team()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> chiamato sull'ultimo mostro del Team 1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.run</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> diventa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Messaggio di vittoria per Giocatore 1.</t>
+    </r>
+  </si>
+  <si>
+    <t>game.run = False</t>
+  </si>
+  <si>
+    <r>
+      <t>Il mostro attivo muore (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>hp=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">). Chiamata a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>switch_turn()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.active_menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> diventa 'change_monster' e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>force_change</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> è True.</t>
+    </r>
+  </si>
+  <si>
+    <t>'change_monster'</t>
+  </si>
+  <si>
+    <t>test_manual_switch_action</t>
+  </si>
+  <si>
+    <r>
+      <t>ChooseMonster(nuovo_mostro).execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> durante il proprio turno.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.selected_monster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cambia. Il menu torna a 'choose_action'.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cambio OK</t>
+  </si>
+  <si>
+    <t>test_target_selection_buff</t>
+  </si>
+  <si>
+    <t>Uso di "Aiuto a casa" (Cura alleato a scelta).</t>
+  </si>
+  <si>
+    <t>Il menu cambia in 'change_monster' per permettere la scelta del target alleato.</t>
+  </si>
+  <si>
+    <t>Scelta target</t>
+  </si>
+  <si>
+    <t>TC-24</t>
+  </si>
+  <si>
+    <t>test_plus_heal_action</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drago (HP=50/150) usa mossa con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>PlusHeal(heal_amount=50)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Il mostro recupera HP dalla mossa base + 50 HP extra dal Plus.</t>
+  </si>
+  <si>
+    <t>HP aumentati</t>
+  </si>
+  <si>
+    <t>TC-25</t>
+  </si>
+  <si>
+    <t>test_plus_damage_action</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Divoratore usa mossa con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>PlusDamage(dmg_amount=40)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Viene applicato un secondo calcolo del danno basato su 40 di potenza extra.</t>
+  </si>
+  <si>
+    <t>Danno extra applicato</t>
+  </si>
+  <si>
+    <t>TC-26</t>
+  </si>
+  <si>
+    <t>test_plus_duration_countdown</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fine del turno con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>active_plus_durations[0] = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il contatore scende a 0 e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>teams_xp[0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> viene resettato a 0.</t>
+    </r>
+  </si>
+  <si>
+    <t>Reset XP OK</t>
+  </si>
+  <si>
+    <t>TC-27</t>
+  </si>
+  <si>
+    <t>test_animation_lock_input</t>
+  </si>
+  <si>
+    <r>
+      <t>game.is_in_animation = True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Pressione tasto.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>buttons_check_input(event)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> non viene eseguito (input bloccati).</t>
+    </r>
+  </si>
+  <si>
+    <t>Nessuna azione</t>
+  </si>
+  <si>
+    <t>TC-28</t>
+  </si>
+  <si>
+    <t>test_death_animation_trigger</t>
+  </si>
+  <si>
+    <r>
+      <t>monster.check_death()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> restituisce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chiamata a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>animation_manager.add_death_anim()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Animazione aggiunta</t>
+  </si>
+  <si>
+    <t>TC-29</t>
+  </si>
+  <si>
+    <t>test_switch_sides_logic</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fine animazione </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>switching_sides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gli sprite di </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>selected_monster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>enemy_monster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> si scambiano di posto.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scambio visivo OK</t>
+  </si>
+  <si>
+    <t>TC-30</t>
+  </si>
+  <si>
+    <t>test_back_button_navigation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Esecuzione </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>Back_to_choose_action.execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.active_menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> torna a 'choose_action' e i bottoni vengono aggiornati.</t>
+    </r>
+  </si>
+  <si>
+    <t>Menu ripristinato</t>
+  </si>
+  <si>
+    <t>TC-31</t>
+  </si>
+  <si>
+    <t>test_monster_stat_min_limit</t>
+  </si>
+  <si>
+    <t>Debuff applicato ad attacco già molto basso.</t>
+  </si>
+  <si>
+    <r>
+      <t>atk_mult</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> non scende mai sotto -1.0 (l'attacco non diventa negativo).</t>
+    </r>
+  </si>
+  <si>
+    <t>Attacco &gt;= 0</t>
+  </si>
+  <si>
+    <t>TC-32</t>
+  </si>
+  <si>
+    <t>test_move_description_render</t>
+  </si>
+  <si>
+    <t>Selezione mossa "Palla di fuoco" nel menu.</t>
+  </si>
+  <si>
+    <r>
+      <t>generate_move_desc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> crea la stringa "30 danno al nemico." sulla superficie dedicata.</t>
+    </r>
+  </si>
+  <si>
+    <t>Descrizione corretta</t>
+  </si>
+  <si>
+    <t>TC-33</t>
+  </si>
+  <si>
+    <t>test_escape_quit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pressione tasto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>K_ESCAPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>game.run</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> impostato a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Chiusura gioco</t>
+  </si>
+  <si>
+    <t>TC-34</t>
+  </si>
+  <si>
+    <t>test_draft_grayscale_logic</t>
+  </si>
+  <si>
+    <t>L'immagine del mostro selezionato nel draft diventa in scala di grigi (metodo luminosity).</t>
+  </si>
+  <si>
+    <t>Immagine Gray</t>
+  </si>
+  <si>
+    <t>TC-35</t>
+  </si>
+  <si>
+    <t>test_draft_button_deactivation</t>
+  </si>
+  <si>
+    <r>
+      <t>DraftButton.activate()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> chiamato su bottone già usato.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>activable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> diventa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e non è più possibile selezionare quel mostro.</t>
+    </r>
+  </si>
+  <si>
+    <t>Disabilitato</t>
+  </si>
+  <si>
+    <t>TC-36</t>
+  </si>
+  <si>
+    <t>test_team_limit_max_draft</t>
+  </si>
+  <si>
+    <r>
+      <t>add_monster_to_team()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> quando il team è pieno.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>match_start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> diventa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e il menu passa a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>choose_action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Match avviato</t>
+  </si>
+  <si>
+    <t>TC-37</t>
+  </si>
+  <si>
+    <t>test_monster_init_stats_drago</t>
+  </si>
+  <si>
+    <r>
+      <t>monster_factory.create_drago(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>HP=150, Att=20, Dif=35, team=0.</t>
+  </si>
+  <si>
+    <t>Stats OK</t>
+  </si>
+  <si>
+    <t>TC-38</t>
+  </si>
+  <si>
+    <t>test_monster_init_stats_serpe</t>
+  </si>
+  <si>
+    <r>
+      <t>monster_factory.create_serpe(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>HP=120, Att=50, Dif=25, team=1.</t>
+  </si>
+  <si>
+    <t>TC-39</t>
+  </si>
+  <si>
+    <t>test_monster_init_stats_divoratore</t>
+  </si>
+  <si>
+    <r>
+      <t>monster_factory.create_divoratore(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>HP=80, Att=100, Dif=15, team=0.</t>
+  </si>
+  <si>
+    <t>TC-40</t>
+  </si>
+  <si>
+    <t>test_plus_debuff_application</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Uso mossa Plus con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>PlusDebuff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (es. Calura+).</t>
+    </r>
+  </si>
+  <si>
+    <t>Applica il debuff base del mostro + un secondo effetto di stato specificato nel Plus.</t>
+  </si>
+  <si>
+    <t>Doppio Debuff</t>
+  </si>
+  <si>
+    <t>TC-41</t>
+  </si>
+  <si>
+    <t>test_plus_remove_debuffs_logic</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mostro con 2 buff e 2 debuff usa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>PlusRemoveDebuffs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La lista </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>status_effects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> contiene solo i 2 buff (power &gt; 0).</t>
+    </r>
+  </si>
+  <si>
+    <t>Solo Buff rimasti</t>
+  </si>
+  <si>
+    <t>TC-42</t>
+  </si>
+  <si>
+    <t>test_dynamic_button_spacing</t>
+  </si>
+  <si>
+    <r>
+      <t>Creazione menu con 5 mostri (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>create_change_monster_buttons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>spacing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tra i bottoni viene ricalcolato dinamicamente per adattarsi allo schermo.</t>
+    </r>
+  </si>
+  <si>
+    <t>Layout OK</t>
+  </si>
+  <si>
+    <t>TC-43</t>
+  </si>
+  <si>
+    <t>test_status_effect_duration_end</t>
+  </si>
+  <si>
+    <t>Turni di un effetto arrivano a 0.</t>
+  </si>
+  <si>
+    <r>
+      <t>se.active</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> diventa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e l'effetto viene rimosso al prossimo aggiornamento.</t>
+    </r>
+  </si>
+  <si>
+    <t>Effetto scaduto</t>
+  </si>
+  <si>
+    <t>TC-44</t>
+  </si>
+  <si>
+    <t>test_defense_buff_scaling</t>
+  </si>
+  <si>
+    <t>Mostro con Difesa 20 riceve Buff 50%.</t>
+  </si>
+  <si>
+    <r>
+      <t>self.defense</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> calcolata a 30 durante il turno.</t>
+    </r>
+  </si>
+  <si>
+    <t>TC-45</t>
+  </si>
+  <si>
+    <t>test_heal_any_ally_selection</t>
+  </si>
+  <si>
+    <r>
+      <t>ChooseMonster_to_buff.execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> su alleato.</t>
+    </r>
+  </si>
+  <si>
+    <t>La cura viene applicata all'alleato selezionato e non al mostro attivo.</t>
+  </si>
+  <si>
+    <t>Cura applicata</t>
+  </si>
+  <si>
+    <t>TC-46</t>
+  </si>
+  <si>
+    <t>test_game_initialization_assets</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chiamata </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>game.set_initiation()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Caricamento corretto di </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>MENU_LAYOUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>animation_manager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>game_bar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Init OK</t>
+  </si>
+  <si>
+    <t>TC-47</t>
+  </si>
+  <si>
+    <t>test_invalid_monster_creation</t>
+  </si>
+  <si>
+    <r>
+      <t>monster_factory.create_monster('Inesistente', 0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Viene sollevato un </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ("Questo mostro non esiste").</t>
+    </r>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>TC-48</t>
+  </si>
+  <si>
+    <t>test_move_desc_text_wrapping</t>
+  </si>
+  <si>
+    <t>Descrizione mossa molto lunga (es. mossa Plus).</t>
+  </si>
+  <si>
+    <r>
+      <t>Il testo viene diviso in più righe (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>lines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) per non uscire dalla </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>move_desc_surf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Testo a capo OK</t>
+  </si>
+  <si>
+    <t>TC-49</t>
+  </si>
+  <si>
+    <t>test_turn_indicator_color</t>
+  </si>
+  <si>
+    <t>Cambio turno da Giocatore 1 a Giocatore 2.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il colore della </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>turn_surface</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cambia da blu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>(0,0,255)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a rosso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>(255,0,0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Colore aggiornato</t>
+  </si>
+  <si>
+    <t>TC-50</t>
+  </si>
+  <si>
+    <t>test_match_start_first_selection</t>
+  </si>
+  <si>
+    <r>
+      <t>Inizio match (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>start_match</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>selected_monster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> è il primo del team 0, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>enemy_monster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> è il primo del team 1.</t>
+    </r>
+  </si>
+  <si>
+    <t>Selezione OK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Esecuzione </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF444746"/>
+        <rFont val="Google Sans Text"/>
+        <family val="2"/>
+      </rPr>
+      <t>DraftButton.activate()</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +2431,36 @@
       <color rgb="FF444746"/>
       <name val="Google Sans Text"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF444746"/>
+      <name val="Google Sans Text"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -655,7 +2509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -687,8 +2541,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -697,6 +2550,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -977,19 +2843,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="29.77734375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="29.44140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.2" thickBot="1">
@@ -1125,7 +2991,7 @@
       <c r="D7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -1159,13 +3025,13 @@
       <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1179,7 +3045,7 @@
       <c r="B10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1249,6 +3115,766 @@
         <v>60</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="42" thickBot="1">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="42" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="42" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42" thickBot="1">
+      <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="14">
+        <v>120</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="42" thickBot="1">
+      <c r="A21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42" thickBot="1">
+      <c r="A22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="42" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="42" thickBot="1">
+      <c r="A25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="42" thickBot="1">
+      <c r="A27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="42" thickBot="1">
+      <c r="A28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="41.4" thickBot="1">
+      <c r="A29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="42" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="42" thickBot="1">
+      <c r="A32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A33" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1">
+      <c r="A34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="18" customFormat="1" ht="55.8" thickBot="1">
+      <c r="A35" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="42" thickBot="1">
+      <c r="A36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="42" thickBot="1">
+      <c r="A37" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A40" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="42" thickBot="1">
+      <c r="A42" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A43" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="42" thickBot="1">
+      <c r="A44" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" s="14">
+        <v>30</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="42" thickBot="1">
+      <c r="A46" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A47" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="42" thickBot="1">
+      <c r="A48" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="42" thickBot="1">
+      <c r="A49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="42" thickBot="1">
+      <c r="A50" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="42" thickBot="1">
+      <c r="A51" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F51" s="14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>